<commit_message>
Update output Excel files.
</commit_message>
<xml_diff>
--- a/documents/schedule_teachers.xlsx
+++ b/documents/schedule_teachers.xlsx
@@ -2356,7 +2356,7 @@
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="11" customWidth="1" min="8" max="8"/>
     <col width="7" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
@@ -2372,7 +2372,7 @@
     <col width="11" customWidth="1" min="20" max="20"/>
     <col width="7" customWidth="1" min="21" max="21"/>
     <col width="13" customWidth="1" min="22" max="22"/>
-    <col width="6" customWidth="1" min="23" max="23"/>
+    <col width="7" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12172,7 +12172,7 @@
     <col width="11" customWidth="1" min="8" max="8"/>
     <col width="7" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
-    <col width="6" customWidth="1" min="11" max="11"/>
+    <col width="7" customWidth="1" min="11" max="11"/>
     <col width="11" customWidth="1" min="12" max="12"/>
     <col width="7" customWidth="1" min="13" max="13"/>
     <col width="13" customWidth="1" min="14" max="14"/>
@@ -18914,7 +18914,7 @@
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="7" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="6" customWidth="1" min="11" max="11"/>
     <col width="12" customWidth="1" min="12" max="12"/>
     <col width="7" customWidth="1" min="13" max="13"/>
     <col width="12" customWidth="1" min="14" max="14"/>
@@ -18926,7 +18926,7 @@
     <col width="12" customWidth="1" min="20" max="20"/>
     <col width="7" customWidth="1" min="21" max="21"/>
     <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="6" customWidth="1" min="23" max="23"/>
+    <col width="7" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -34980,7 +34980,7 @@
     <col width="12" customWidth="1" min="16" max="16"/>
     <col width="7" customWidth="1" min="17" max="17"/>
     <col width="11" customWidth="1" min="18" max="18"/>
-    <col width="7" customWidth="1" min="19" max="19"/>
+    <col width="6" customWidth="1" min="19" max="19"/>
     <col width="12" customWidth="1" min="20" max="20"/>
     <col width="7" customWidth="1" min="21" max="21"/>
     <col width="12" customWidth="1" min="22" max="22"/>

</xml_diff>